<commit_message>
merge and revert package dependencies
</commit_message>
<xml_diff>
--- a/src/data/summer21/leadership_summer21.xlsx
+++ b/src/data/summer21/leadership_summer21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyenokida/Projects/dspuci-website-gatsby/src/data/summer21/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00703872-464C-3641-AB2A-2E6713F7D157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF7EA5D-B14B-0848-922E-C5660B9324EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39720" yWindow="-1000" windowWidth="28800" windowHeight="17500" xr2:uid="{2C0ED811-1999-2046-A233-A574ADF233C5}"/>
+    <workbookView xWindow="49240" yWindow="120" windowWidth="28800" windowHeight="17500" xr2:uid="{2C0ED811-1999-2046-A233-A574ADF233C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -112,14 +112,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <u/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -467,96 +466,96 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated to  Winter/Spring 2022 EC
</commit_message>
<xml_diff>
--- a/src/data/summer21/leadership_summer21.xlsx
+++ b/src/data/summer21/leadership_summer21.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brennenwong/Documents/DSP Website/src/data/summer21/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56512EC1-4F0B-DC45-AA86-232246D6C498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B9D3D1-A1BF-C54D-B8B7-936F4DDB8DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" xr2:uid="{2C0ED811-1999-2046-A233-A574ADF233C5}"/>
   </bookViews>
@@ -69,34 +69,34 @@
     <t>Vice President of Alumni Relations</t>
   </si>
   <si>
-    <t>Jocelyn Kuo</t>
-  </si>
-  <si>
     <t>Megha Bhargava</t>
   </si>
   <si>
-    <t>Patrick Tu</t>
-  </si>
-  <si>
-    <t>Aarti Vellimedu</t>
-  </si>
-  <si>
-    <t>Jessie Yang</t>
-  </si>
-  <si>
     <t>Grace Till</t>
   </si>
   <si>
     <t>Kevin Cao</t>
   </si>
   <si>
-    <t>Aishu Parsuram</t>
-  </si>
-  <si>
-    <t>Mohit Shah</t>
-  </si>
-  <si>
     <t>Grace Hsiang</t>
+  </si>
+  <si>
+    <t>Aayush Shah</t>
+  </si>
+  <si>
+    <t>Dylan Tanzil</t>
+  </si>
+  <si>
+    <t>Tiffany Than</t>
+  </si>
+  <si>
+    <t>Alex Pham</t>
+  </si>
+  <si>
+    <t>Tommy Truong</t>
+  </si>
+  <si>
+    <t>Sean Devine</t>
   </si>
 </sst>
 </file>
@@ -466,7 +466,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D13" activeCellId="1" sqref="C11 D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -481,7 +481,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -489,7 +489,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
@@ -497,7 +497,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -505,7 +505,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
@@ -513,7 +513,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
@@ -521,7 +521,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
@@ -529,7 +529,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>8</v>
@@ -537,7 +537,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
@@ -545,7 +545,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>10</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>11</v>

</xml_diff>